<commit_message>
Modification de textes dans le backoffice et dans le fichier modèle
</commit_message>
<xml_diff>
--- a/modele.xlsx
+++ b/modele.xlsx
@@ -75,18 +75,12 @@
     <t>Date Edition originale</t>
   </si>
   <si>
-    <t>retranscription de l'Envoi</t>
-  </si>
-  <si>
     <t>Illustration</t>
   </si>
   <si>
     <t>description matérielle</t>
   </si>
   <si>
-    <t>Annotations- marques par l'artiste</t>
-  </si>
-  <si>
     <t>Commentaire issu de la source</t>
   </si>
   <si>
@@ -154,6 +148,12 @@
   </si>
   <si>
     <t>Remarque</t>
+  </si>
+  <si>
+    <t>Mention de l'envoi</t>
+  </si>
+  <si>
+    <t>Marques de lecture</t>
   </si>
 </sst>
 </file>
@@ -500,7 +500,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -572,7 +572,7 @@
         <v>10</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>11</v>
@@ -587,40 +587,40 @@
         <v>18</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="W1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:32">
@@ -631,49 +631,49 @@
         <v>38</v>
       </c>
       <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" t="s">
         <v>31</v>
       </c>
-      <c r="D2" t="s">
+      <c r="M2" t="s">
         <v>32</v>
-      </c>
-      <c r="E2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L2" t="s">
-        <v>33</v>
-      </c>
-      <c r="M2" t="s">
-        <v>34</v>
       </c>
       <c r="N2">
         <v>1854</v>
       </c>
       <c r="P2" t="s">
+        <v>34</v>
+      </c>
+      <c r="U2" t="s">
+        <v>33</v>
+      </c>
+      <c r="X2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y2" t="s">
         <v>36</v>
       </c>
-      <c r="U2" t="s">
+      <c r="AA2" t="s">
         <v>35</v>
       </c>
-      <c r="X2" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA2" t="s">
+      <c r="AC2" t="s">
         <v>37</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>39</v>
       </c>
-      <c r="AD2" t="s">
-        <v>41</v>
-      </c>
       <c r="AE2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="AF2">
         <v>1</v>

</xml_diff>

<commit_message>
Modification sur le modèle XLS : masquage de la première colonne
</commit_message>
<xml_diff>
--- a/modele.xlsx
+++ b/modele.xlsx
@@ -500,12 +500,12 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W2" sqref="W2"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="21.140625" customWidth="1"/>
     <col min="4" max="4" width="21.5703125" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" customWidth="1"/>

</xml_diff>

<commit_message>
Modifications sur les entêtes du fichier modèle
</commit_message>
<xml_diff>
--- a/modele.xlsx
+++ b/modele.xlsx
@@ -99,9 +99,6 @@
     <t>ARK Iframe</t>
   </si>
   <si>
-    <t>Type de notice. 1 : La notice et l'iframe sont de la même édition / 2 : La notice et l’iframe ne sont pas de la même édition / 3 : La notice est la même édition et l’iframe n’est pas la même édition / 4 : Iframe uniquement</t>
-  </si>
-  <si>
     <t>Genre (référencetiel Rameau)</t>
   </si>
   <si>
@@ -154,6 +151,9 @@
   </si>
   <si>
     <t>Marques de lecture</t>
+  </si>
+  <si>
+    <t>Type de notice. 1 : La notice et l'iframe sont de la même édition / 2 : La notice et l’iframe ne sont pas de la même édition / 3 : La notice est la même édition et l’iframe n’est pas la même édition / 4 : Iframe uniquement / 5 : Iframe d'une édition approchante uniquement / 6 : Notice de la même édition uniquement / 7 : Notice d'une édition approchante uniquement</t>
   </si>
 </sst>
 </file>
@@ -197,9 +197,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -498,9 +501,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AF2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="AF1" sqref="AF1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -525,7 +528,7 @@
     <col min="33" max="33" width="36.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="1" customFormat="1" ht="52.5" customHeight="1">
+    <row r="1" spans="1:32" s="1" customFormat="1" ht="130.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -590,10 +593,10 @@
         <v>19</v>
       </c>
       <c r="V1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>21</v>
@@ -605,10 +608,10 @@
         <v>22</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AC1" s="1" t="s">
         <v>24</v>
@@ -619,11 +622,11 @@
       <c r="AE1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AF1" s="1" t="s">
-        <v>27</v>
+      <c r="AF1" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:32">
+    <row r="2" spans="1:32" ht="130.5" customHeight="1">
       <c r="A2">
         <v>1</v>
       </c>
@@ -631,49 +634,49 @@
         <v>38</v>
       </c>
       <c r="C2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" t="s">
         <v>30</v>
       </c>
-      <c r="E2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" t="s">
-        <v>40</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>31</v>
-      </c>
-      <c r="M2" t="s">
-        <v>32</v>
       </c>
       <c r="N2">
         <v>1854</v>
       </c>
       <c r="P2" t="s">
+        <v>33</v>
+      </c>
+      <c r="U2" t="s">
+        <v>32</v>
+      </c>
+      <c r="X2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA2" t="s">
         <v>34</v>
       </c>
-      <c r="U2" t="s">
-        <v>33</v>
-      </c>
-      <c r="X2" t="s">
+      <c r="AC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD2" t="s">
         <v>38</v>
       </c>
-      <c r="Y2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>39</v>
-      </c>
       <c r="AE2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AF2">
         <v>1</v>

</xml_diff>